<commit_message>
Update Análise Financeira PROJ4.xlsx
</commit_message>
<xml_diff>
--- a/Analise Financeira/Análise Financeira PROJ4.xlsx
+++ b/Analise Financeira/Análise Financeira PROJ4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Vitor\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gestao-de-Portfolios\Analise Financeira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69E7AEB-F08E-4DC4-85B9-C48F0800A1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E552852D-E1C5-4629-94ED-6FF3D298E7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showSheetTabs="0" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{5407E0C7-D3D1-4456-BA1C-167F3E5756A9}"/>
+    <workbookView showSheetTabs="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{5407E0C7-D3D1-4456-BA1C-167F3E5756A9}"/>
   </bookViews>
   <sheets>
     <sheet name="APRESENTAÇÃO" sheetId="2" r:id="rId1"/>
@@ -193,10 +193,10 @@
     <t>ANÁLISE</t>
   </si>
   <si>
-    <t>O projeto é financeiramente viável e atrativo, com uma TIR de 12%, bem acima da TMA de 8%, e um payback de 3 anos, indicando recuperação do capital. O VPL positivo e o ROI de 24% reforçam a viabilidade, garantindo retorno significativo. Recomenda-se a aprovação do projeto.</t>
+    <t>Plataforma de Gestão de Requisitos</t>
   </si>
   <si>
-    <t>Plataforma de Gestão de Requisitos</t>
+    <t>O projeto "Plataforma de Gestão de Requisitos" é financeiramente viável, apresentando uma TIR de 12%, que supera a TMA de 11%, indicando que os retornos esperados são superiores à taxa mínima de atratividade. O período de payback é de 3 anos, ou seja, o capital investido será recuperado nesse tempo, o que reforça a atratividade do projeto. Além disso, o VPL positivo de R$ 60.000,00 mostra que os fluxos de caixa descontados superam o investimento inicial, agregando valor ao projeto, enquanto o ROI de 24% demonstra um retorno significativo sobre o investimento. Com esses indicadores, recomenda-se a aprovação do projeto.</t>
   </si>
 </sst>
 </file>
@@ -597,7 +597,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1075,7 +1075,103 @@
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
+      <sheetData sheetId="5">
+        <row r="6">
+          <cell r="D6" t="str">
+            <v>Automóvel</v>
+          </cell>
+          <cell r="F6" t="str">
+            <v>Edificações</v>
+          </cell>
+          <cell r="J6" t="str">
+            <v>Recursos Humanos</v>
+          </cell>
+          <cell r="L6" t="str">
+            <v>Novo</v>
+          </cell>
+          <cell r="N6" t="str">
+            <v>Entrada</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>Computador</v>
+          </cell>
+          <cell r="F7" t="str">
+            <v>Máquinas e Equipamentos</v>
+          </cell>
+          <cell r="J7" t="str">
+            <v>Financeiro</v>
+          </cell>
+          <cell r="L7" t="str">
+            <v>Ótimo</v>
+          </cell>
+          <cell r="N7" t="str">
+            <v>Saída</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="D8" t="str">
+            <v>Sala comercial</v>
+          </cell>
+          <cell r="F8" t="str">
+            <v>Instalações</v>
+          </cell>
+          <cell r="J8" t="str">
+            <v>Tec. Informação</v>
+          </cell>
+          <cell r="L8" t="str">
+            <v>Bom</v>
+          </cell>
+          <cell r="N8" t="str">
+            <v>Perda</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="D9" t="str">
+            <v>Moto</v>
+          </cell>
+          <cell r="F9" t="str">
+            <v>Móveis e Utensílios</v>
+          </cell>
+          <cell r="J9" t="str">
+            <v>Diretoria</v>
+          </cell>
+          <cell r="L9" t="str">
+            <v>Regular</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="D10" t="str">
+            <v>Calculadoras</v>
+          </cell>
+          <cell r="F10" t="str">
+            <v>Veículos</v>
+          </cell>
+          <cell r="J10" t="str">
+            <v>Almoxarifado</v>
+          </cell>
+          <cell r="L10" t="str">
+            <v>Péssimo</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="D11" t="str">
+            <v>Cadeiras</v>
+          </cell>
+          <cell r="F11" t="str">
+            <v>Computadores e Periféricos</v>
+          </cell>
+          <cell r="J11" t="str">
+            <v>Logística</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="D12" t="str">
+            <v>Mesas</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1131,7 +1227,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -1437,9 +1533,9 @@
       <selection pane="bottomLeft" activeCell="A22" sqref="A22:XFD67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1462,7 +1558,7 @@
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
     </row>
-    <row r="2" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1485,7 +1581,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1508,7 +1604,7 @@
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
     </row>
-    <row r="4" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1531,7 +1627,7 @@
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
     </row>
-    <row r="5" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1554,7 +1650,7 @@
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
     </row>
-    <row r="6" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1577,7 +1673,7 @@
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
     </row>
-    <row r="7" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1600,7 +1696,7 @@
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
     </row>
-    <row r="8" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1623,7 +1719,7 @@
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
     </row>
-    <row r="9" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1646,7 +1742,7 @@
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
     </row>
-    <row r="10" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1669,7 +1765,7 @@
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
     </row>
-    <row r="11" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1692,7 +1788,7 @@
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
     </row>
-    <row r="12" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1715,7 +1811,7 @@
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
     </row>
-    <row r="13" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1738,7 +1834,7 @@
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
     </row>
-    <row r="14" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1761,7 +1857,7 @@
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
     </row>
-    <row r="15" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1784,7 +1880,7 @@
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
     </row>
-    <row r="16" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1807,7 +1903,7 @@
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
     </row>
-    <row r="17" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1830,7 +1926,7 @@
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
     </row>
-    <row r="18" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1853,7 +1949,7 @@
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
     </row>
-    <row r="19" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1876,7 +1972,7 @@
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
     </row>
-    <row r="20" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1899,7 +1995,7 @@
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
     </row>
-    <row r="21" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1922,7 +2018,7 @@
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
     </row>
-    <row r="22" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1945,7 +2041,7 @@
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
     </row>
-    <row r="23" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1968,7 +2064,7 @@
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
     </row>
-    <row r="24" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1991,7 +2087,7 @@
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
     </row>
-    <row r="25" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2014,7 +2110,7 @@
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
     </row>
-    <row r="26" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2037,7 +2133,7 @@
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
     </row>
-    <row r="27" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2060,7 +2156,7 @@
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
     </row>
-    <row r="28" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2083,7 +2179,7 @@
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
     </row>
-    <row r="29" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2106,7 +2202,7 @@
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
     </row>
-    <row r="30" spans="1:21" ht="409.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="409.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2129,7 +2225,7 @@
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
     </row>
-    <row r="31" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2166,22 +2262,22 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4:G4"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14:G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="45.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="3.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="45.88671875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -2189,27 +2285,27 @@
       <c r="F2" s="7"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="2:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="4"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="12"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="2:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="33"/>
       <c r="E4" s="33"/>
       <c r="F4" s="33"/>
       <c r="G4" s="34"/>
     </row>
-    <row r="5" spans="2:7" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:7" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:7" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>1</v>
       </c>
@@ -2227,7 +2323,7 @@
       </c>
       <c r="G6" s="27"/>
     </row>
-    <row r="7" spans="2:7" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10">
         <v>0</v>
       </c>
@@ -2250,7 +2346,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="10">
         <v>1</v>
       </c>
@@ -2259,20 +2355,20 @@
       </c>
       <c r="D8" s="13">
         <f t="shared" ref="D8:D19" si="0">PV($G$8,B8,,-C8)</f>
-        <v>46296.296296296292</v>
+        <v>45045.045045045044</v>
       </c>
       <c r="E8" s="13">
         <f>D8+E7</f>
-        <v>-203703.70370370371</v>
+        <v>-204954.95495495497</v>
       </c>
       <c r="F8" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="18">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="10">
         <v>2</v>
       </c>
@@ -2281,11 +2377,11 @@
       </c>
       <c r="D9" s="13">
         <f t="shared" si="0"/>
-        <v>60013.71742112482</v>
+        <v>56813.570327083835</v>
       </c>
       <c r="E9" s="13">
         <f t="shared" ref="E9:E19" si="1">D9+E8</f>
-        <v>-143689.9862825789</v>
+        <v>-148141.38462787113</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>8</v>
@@ -2294,7 +2390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="10">
         <v>3</v>
       </c>
@@ -2303,11 +2399,11 @@
       </c>
       <c r="D10" s="13">
         <f t="shared" si="0"/>
-        <v>71444.901691815263</v>
+        <v>65807.224317085522</v>
       </c>
       <c r="E10" s="13">
         <f t="shared" si="1"/>
-        <v>-72245.084590763639</v>
+        <v>-82334.160310785606</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>9</v>
@@ -2316,7 +2412,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="10">
         <v>4</v>
       </c>
@@ -2325,11 +2421,11 @@
       </c>
       <c r="D11" s="13">
         <f t="shared" si="0"/>
-        <v>73502.98527964532</v>
+        <v>65873.097414500007</v>
       </c>
       <c r="E11" s="13">
         <f t="shared" si="1"/>
-        <v>1257.9006888816803</v>
+        <v>-16461.062896285599</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>10</v>
@@ -2338,7 +2434,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="10">
         <v>5</v>
       </c>
@@ -2347,11 +2443,11 @@
       </c>
       <c r="D12" s="13">
         <f t="shared" si="0"/>
-        <v>81669.983644050357</v>
+        <v>71214.159367027038</v>
       </c>
       <c r="E12" s="13">
         <f t="shared" si="1"/>
-        <v>82927.884332932037</v>
+        <v>54753.096470741439</v>
       </c>
       <c r="F12" s="22" t="s">
         <v>11</v>
@@ -2360,7 +2456,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="10">
         <v>6</v>
       </c>
@@ -2371,14 +2467,14 @@
       </c>
       <c r="E13" s="21">
         <f t="shared" si="1"/>
-        <v>82927.884332932037</v>
+        <v>54753.096470741439</v>
       </c>
       <c r="F13" s="26" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="27"/>
     </row>
-    <row r="14" spans="2:7" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="10">
         <v>7</v>
       </c>
@@ -2389,14 +2485,14 @@
       </c>
       <c r="E14" s="21">
         <f t="shared" si="1"/>
-        <v>82927.884332932037</v>
+        <v>54753.096470741439</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G14" s="29"/>
     </row>
-    <row r="15" spans="2:7" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="10">
         <v>8</v>
       </c>
@@ -2407,12 +2503,12 @@
       </c>
       <c r="E15" s="21">
         <f t="shared" si="1"/>
-        <v>82927.884332932037</v>
+        <v>54753.096470741439</v>
       </c>
       <c r="F15" s="28"/>
       <c r="G15" s="29"/>
     </row>
-    <row r="16" spans="2:7" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="10">
         <v>9</v>
       </c>
@@ -2423,12 +2519,12 @@
       </c>
       <c r="E16" s="21">
         <f t="shared" si="1"/>
-        <v>82927.884332932037</v>
+        <v>54753.096470741439</v>
       </c>
       <c r="F16" s="28"/>
       <c r="G16" s="29"/>
     </row>
-    <row r="17" spans="2:7" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="10">
         <v>10</v>
       </c>
@@ -2439,12 +2535,12 @@
       </c>
       <c r="E17" s="21">
         <f t="shared" si="1"/>
-        <v>82927.884332932037</v>
+        <v>54753.096470741439</v>
       </c>
       <c r="F17" s="28"/>
       <c r="G17" s="29"/>
     </row>
-    <row r="18" spans="2:7" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="10">
         <v>11</v>
       </c>
@@ -2455,12 +2551,12 @@
       </c>
       <c r="E18" s="21">
         <f t="shared" si="1"/>
-        <v>82927.884332932037</v>
+        <v>54753.096470741439</v>
       </c>
       <c r="F18" s="28"/>
       <c r="G18" s="29"/>
     </row>
-    <row r="19" spans="2:7" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="10">
         <v>12</v>
       </c>
@@ -2471,12 +2567,12 @@
       </c>
       <c r="E19" s="21">
         <f t="shared" si="1"/>
-        <v>82927.884332932037</v>
+        <v>54753.096470741439</v>
       </c>
       <c r="F19" s="30"/>
       <c r="G19" s="31"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
     </row>
   </sheetData>
@@ -2505,11 +2601,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3762cdab-2681-44c0-9739-9df1020ff737" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2708,20 +2805,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3762cdab-2681-44c0-9739-9df1020ff737" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A9B4C68-9AAE-487A-961A-7DBE3ECBAE68}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B3CF0F-FAB6-49F6-AC88-4CE8A1927A13}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3762cdab-2681-44c0-9739-9df1020ff737"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2746,9 +2840,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B3CF0F-FAB6-49F6-AC88-4CE8A1927A13}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A9B4C68-9AAE-487A-961A-7DBE3ECBAE68}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3762cdab-2681-44c0-9739-9df1020ff737"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>